<commit_message>
update buku dan ppt
</commit_message>
<xml_diff>
--- a/Uji Coba/hasil.xlsx
+++ b/Uji Coba/hasil.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -338,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -398,6 +398,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,6 +461,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -553,11 +560,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="728300576"/>
-        <c:axId val="728301120"/>
+        <c:axId val="-1664634576"/>
+        <c:axId val="-1664633488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="728300576"/>
+        <c:axId val="-1664634576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +606,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="728301120"/>
+        <c:crossAx val="-1664633488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -607,7 +614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="728301120"/>
+        <c:axId val="-1664633488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +665,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="728300576"/>
+        <c:crossAx val="-1664634576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1032,11 +1039,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="728302752"/>
-        <c:axId val="728303840"/>
+        <c:axId val="-1664640016"/>
+        <c:axId val="-1664634032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="728302752"/>
+        <c:axId val="-1664640016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1142,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="728303840"/>
+        <c:crossAx val="-1664634032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1143,7 +1150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="728303840"/>
+        <c:axId val="-1664634032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1255,7 +1262,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="728302752"/>
+        <c:crossAx val="-1664640016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1530,11 +1537,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="728308192"/>
-        <c:axId val="728308736"/>
+        <c:axId val="-1664637840"/>
+        <c:axId val="-1446209440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="728308192"/>
+        <c:axId val="-1664637840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1632,7 +1639,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="728308736"/>
+        <c:crossAx val="-1446209440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1640,7 +1647,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="728308736"/>
+        <c:axId val="-1446209440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,7 +1759,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="728308192"/>
+        <c:crossAx val="-1664637840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1976,11 +1983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="890514320"/>
-        <c:axId val="890520848"/>
+        <c:axId val="-1446212160"/>
+        <c:axId val="-1446211616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="890514320"/>
+        <c:axId val="-1446212160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,7 +2085,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="890520848"/>
+        <c:crossAx val="-1446211616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2086,7 +2093,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="890520848"/>
+        <c:axId val="-1446211616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2200,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="890514320"/>
+        <c:crossAx val="-1446212160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2385,11 +2392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="890508336"/>
-        <c:axId val="890508880"/>
+        <c:axId val="-1446201824"/>
+        <c:axId val="-1446204544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="890508336"/>
+        <c:axId val="-1446201824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,7 +2494,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="890508880"/>
+        <c:crossAx val="-1446204544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2495,7 +2502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="890508880"/>
+        <c:axId val="-1446204544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2602,7 +2609,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="890508336"/>
+        <c:crossAx val="-1446201824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2818,11 +2825,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="965090672"/>
-        <c:axId val="965091216"/>
+        <c:axId val="-1446215424"/>
+        <c:axId val="-1446205088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="965090672"/>
+        <c:axId val="-1446215424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2921,7 +2928,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="965091216"/>
+        <c:crossAx val="-1446205088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2929,7 +2936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="965091216"/>
+        <c:axId val="-1446205088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3036,7 +3043,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="965090672"/>
+        <c:crossAx val="-1446215424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3252,11 +3259,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="965051152"/>
-        <c:axId val="965051696"/>
+        <c:axId val="-1446205632"/>
+        <c:axId val="-1446204000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="965051152"/>
+        <c:axId val="-1446205632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3355,7 +3362,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="965051696"/>
+        <c:crossAx val="-1446204000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3363,7 +3370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="965051696"/>
+        <c:axId val="-1446204000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3475,7 +3482,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="965051152"/>
+        <c:crossAx val="-1446205632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3818,11 +3825,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="965089040"/>
-        <c:axId val="965093936"/>
+        <c:axId val="-1506481936"/>
+        <c:axId val="-1506478672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="965089040"/>
+        <c:axId val="-1506481936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3925,7 +3932,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="965093936"/>
+        <c:crossAx val="-1506478672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3933,7 +3940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="965093936"/>
+        <c:axId val="-1506478672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4040,7 +4047,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="965089040"/>
+        <c:crossAx val="-1506481936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4415,11 +4422,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="890515952"/>
-        <c:axId val="890509424"/>
+        <c:axId val="-1506482480"/>
+        <c:axId val="-1506481392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="890515952"/>
+        <c:axId val="-1506482480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4523,7 +4530,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="890509424"/>
+        <c:crossAx val="-1506481392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4531,7 +4538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="890509424"/>
+        <c:axId val="-1506481392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4638,7 +4645,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="890515952"/>
+        <c:crossAx val="-1506482480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10135,10 +10142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q165"/>
+  <dimension ref="A1:Q194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B158" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172"/>
+    <sheetView tabSelected="1" topLeftCell="A182" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D186" sqref="D186:D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11827,6 +11834,79 @@
       </c>
       <c r="F165">
         <v>57.5</v>
+      </c>
+    </row>
+    <row r="185" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="186" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186" s="23">
+        <v>110.8</v>
+      </c>
+    </row>
+    <row r="187" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C187">
+        <v>2</v>
+      </c>
+      <c r="D187" s="24">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="188" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C188">
+        <v>3</v>
+      </c>
+      <c r="D188" s="24">
+        <v>268.39999999999998</v>
+      </c>
+    </row>
+    <row r="189" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C189">
+        <v>4</v>
+      </c>
+      <c r="D189" s="24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="190" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C190">
+        <v>5</v>
+      </c>
+      <c r="D190" s="24">
+        <v>75.8</v>
+      </c>
+    </row>
+    <row r="191" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C191">
+        <v>6</v>
+      </c>
+      <c r="D191" s="24">
+        <v>78.400000000000006</v>
+      </c>
+    </row>
+    <row r="192" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C192">
+        <v>7</v>
+      </c>
+      <c r="D192" s="24">
+        <v>60.8</v>
+      </c>
+    </row>
+    <row r="193" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C193">
+        <v>8</v>
+      </c>
+      <c r="D193" s="24">
+        <v>151.19999999999999</v>
+      </c>
+    </row>
+    <row r="194" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C194">
+        <v>9</v>
+      </c>
+      <c r="D194" s="24">
+        <v>100.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>